<commit_message>
ajout assets et credentials
</commit_message>
<xml_diff>
--- a/04-Dispatcher/Data/Config.xlsx
+++ b/04-Dispatcher/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -157,6 +157,24 @@
   </si>
   <si>
     <t xml:space="preserve">Description (Assets will always overwrite other config)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url_seLoger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url_seLoger </t>
+  </si>
+  <si>
+    <t xml:space="preserve">logement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url de SeLoger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">url_helloPret </t>
+  </si>
+  <si>
+    <t xml:space="preserve">url de helloPret</t>
   </si>
 </sst>
 </file>
@@ -287,11 +305,11 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43"/>
@@ -1360,8 +1378,8 @@
     <row r="998" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1380,7 +1398,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51"/>
@@ -1551,7 +1569,7 @@
       <c r="A17" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="0" t="b">
+      <c r="B17" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2532,8 +2550,8 @@
     <row r="988" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2548,16 +2566,16 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="65.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="65.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2596,8 +2614,34 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3597,8 +3641,8 @@
     <row r="1000" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
etape intermediaire creation assets
</commit_message>
<xml_diff>
--- a/04-Dispatcher/Data/Config.xlsx
+++ b/04-Dispatcher/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t xml:space="preserve">url de helloPret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">str_batchName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nom du batch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bol_containError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">presence erreur dans le batch</t>
   </si>
 </sst>
 </file>
@@ -309,7 +321,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43"/>
@@ -1378,8 +1390,8 @@
     <row r="998" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1398,7 +1410,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51"/>
@@ -2550,8 +2562,8 @@
     <row r="988" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2567,10 +2579,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.1"/>
@@ -2642,8 +2654,34 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3641,8 +3679,8 @@
     <row r="1000" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>